<commit_message>
Added environment type to tier configuration requests
</commit_message>
<xml_diff>
--- a/reports/tier_configuration_requests/template.xlsx
+++ b/reports/tier_configuration_requests/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/cnctcli/reports/connect-reports/reports/tier_configuration_requests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9BA860-D065-114A-8882-25FECE413E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3472F32-D1B1-DF41-9D8E-4B357C61B724}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36260" yWindow="500" windowWidth="35840" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AA$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AB$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Request ID</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Parent Configuration ID</t>
+  </si>
+  <si>
+    <t>Environment</t>
   </si>
 </sst>
 </file>
@@ -145,9 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -461,29 +466,29 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="4" width="21.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="7" width="21.1640625" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="21.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="45.83203125" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="45.83203125" customWidth="1"/>
-    <col min="21" max="21" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="45.83203125" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="45.83203125" customWidth="1"/>
-    <col min="25" max="26" width="15.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="45.83203125" customWidth="1"/>
+    <col min="5" max="8" width="21.1640625" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="19.33203125" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="21.1640625" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="45.83203125" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="45.83203125" customWidth="1"/>
+    <col min="22" max="22" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="45.83203125" customWidth="1"/>
+    <col min="24" max="24" width="15" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="45.83203125" customWidth="1"/>
+    <col min="26" max="27" width="15.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,71 +508,74 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
+  <autoFilter ref="A1:AB1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>